<commit_message>
Updated Excel tabel with queries
</commit_message>
<xml_diff>
--- a/backend/queries_by_difficulty.xlsx
+++ b/backend/queries_by_difficulty.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\laure\OneDrive\Documents\University\8_Semester\BA\Covbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lstampfl/Dropbox/Mac/Documents/University/8_Semester/BA/Covbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E881292-4699-4847-B2AA-332A9F645D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A579850-4604-D148-B12C-E97A1BAECC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{23BBDD8F-E7EB-45C8-AE03-40A229D24D6C}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{23BBDD8F-E7EB-45C8-AE03-40A229D24D6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -628,17 +628,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854A03FF-80A6-4AF0-8B30-213E9069B8D1}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.06640625" customWidth="1"/>
+    <col min="1" max="1" width="61" customWidth="1"/>
     <col min="10" max="10" width="140.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -649,7 +649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -668,7 +668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -679,7 +679,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -687,7 +687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -698,7 +698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -709,7 +709,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -731,7 +731,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
@@ -742,7 +742,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -753,7 +753,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -764,7 +764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
@@ -772,7 +772,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>21</v>
       </c>
@@ -780,7 +780,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>22</v>
       </c>
@@ -791,7 +791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -799,7 +799,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -807,7 +807,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -815,7 +815,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -826,7 +826,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -837,7 +837,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -845,7 +845,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -856,7 +856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -867,24 +867,24 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
       <c r="I26">
@@ -894,8 +894,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I27">
@@ -905,8 +905,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
       <c r="I28">
@@ -916,7 +916,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="I29">
         <v>1</v>
       </c>
@@ -924,7 +927,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="1" t="s">
+        <v>41</v>
+      </c>
       <c r="I30">
         <v>1</v>
       </c>
@@ -932,7 +938,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>47</v>
+      </c>
       <c r="I31">
         <v>1</v>
       </c>
@@ -940,17 +949,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>40</v>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="J32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>41</v>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -959,9 +968,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>47</v>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="I34">
         <v>1</v>
@@ -970,9 +979,9 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>48</v>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="I35">
         <v>1</v>
@@ -981,9 +990,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>49</v>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="I36">
         <v>1</v>
@@ -992,9 +1001,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>50</v>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="I37">
         <v>1</v>
@@ -1003,18 +1012,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I39">
         <v>1</v>
       </c>
@@ -1022,10 +1025,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>53</v>
-      </c>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I40">
         <v>1</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>54</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>55</v>
       </c>
@@ -1055,7 +1055,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -1071,7 +1071,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>60</v>
       </c>
@@ -1079,7 +1079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>68</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>69</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I50">
         <v>1</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I51">
         <v>1</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I52">
         <v>1</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I53">
         <v>1</v>
       </c>
@@ -1149,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I54">
         <v>1</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I55">
         <v>1</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I56">
         <v>1</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I57">
         <v>1</v>
       </c>
@@ -1181,12 +1181,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J58" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I59">
         <v>1</v>
       </c>
@@ -1194,12 +1194,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J60" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I61">
         <v>1</v>
       </c>
@@ -1207,27 +1207,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J62" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J63" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="J64" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="65" spans="9:10" x14ac:dyDescent="0.2">
       <c r="J65" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="66" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I66">
         <v>1</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I67">
         <v>1</v>
       </c>
@@ -1243,12 +1243,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="68" spans="9:10" x14ac:dyDescent="0.2">
       <c r="J68" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="69" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I69">
         <v>1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="9:10" x14ac:dyDescent="0.45">
+    <row r="70" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I70">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated remaining query annotations
</commit_message>
<xml_diff>
--- a/backend/queries_by_difficulty.xlsx
+++ b/backend/queries_by_difficulty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lstampfl/Dropbox/Mac/Documents/University/8_Semester/BA/Covbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A579850-4604-D148-B12C-E97A1BAECC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4461D3B-8EB1-D242-9E33-B11EF4EE99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{23BBDD8F-E7EB-45C8-AE03-40A229D24D6C}"/>
   </bookViews>
@@ -628,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854A03FF-80A6-4AF0-8B30-213E9069B8D1}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:A37"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated query Excel file
</commit_message>
<xml_diff>
--- a/backend/queries_by_difficulty.xlsx
+++ b/backend/queries_by_difficulty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lstampfl/Dropbox/Mac/Documents/University/8_Semester/BA/Covbot/backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4461D3B-8EB1-D242-9E33-B11EF4EE99F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC28D900-EDA2-934A-996A-160225F7F76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{23BBDD8F-E7EB-45C8-AE03-40A229D24D6C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="70">
   <si>
     <t>How many new cases have been reported in Austria today?</t>
   </si>
@@ -202,9 +202,6 @@
     <t>How many people are vaccinated?</t>
   </si>
   <si>
-    <t>How many people were vaccinated tody?</t>
-  </si>
-  <si>
     <t>How many corona cases got reported today?</t>
   </si>
   <si>
@@ -245,13 +242,16 @@
   </si>
   <si>
     <t>Could you tell me which how many new COVID cases were reported in Austria on 2nd February 2022?</t>
+  </si>
+  <si>
+    <t>How many people were vaccinated today?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +273,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +298,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -301,19 +313,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{854A03FF-80A6-4AF0-8B30-213E9069B8D1}">
   <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -949,11 +964,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="J32" t="s">
+      <c r="J32" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1013,11 +1028,17 @@
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="J38" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="I39">
         <v>1</v>
       </c>
@@ -1026,6 +1047,9 @@
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="I40">
         <v>1</v>
       </c>
@@ -1034,8 +1058,8 @@
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>54</v>
+      <c r="A41" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="I41">
         <v>1</v>
@@ -1045,8 +1069,8 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>55</v>
+      <c r="A42" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="I42">
         <v>1</v>
@@ -1056,49 +1080,40 @@
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>56</v>
+      <c r="A43" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="J43" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>58</v>
+      <c r="A44" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="J44" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>60</v>
+      <c r="A45" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="J45" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>65</v>
-      </c>
-      <c r="J46" t="s">
+      <c r="J46" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>66</v>
-      </c>
       <c r="J47" s="2" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>68</v>
-      </c>
       <c r="I48">
         <v>1</v>
       </c>
@@ -1106,10 +1121,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>69</v>
-      </c>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I49">
         <v>1</v>
       </c>
@@ -1117,7 +1129,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I50">
         <v>1</v>
       </c>
@@ -1125,7 +1137,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I51">
         <v>1</v>
       </c>
@@ -1133,7 +1145,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I52">
         <v>1</v>
       </c>
@@ -1141,7 +1153,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I53">
         <v>1</v>
       </c>
@@ -1149,7 +1161,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I54">
         <v>1</v>
       </c>
@@ -1157,7 +1169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I55">
         <v>1</v>
       </c>
@@ -1165,66 +1177,63 @@
         <v>54</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="9:10" x14ac:dyDescent="0.2">
       <c r="I56">
         <v>1</v>
       </c>
       <c r="J56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I57">
-        <v>1</v>
-      </c>
-      <c r="J57" t="s">
+    <row r="58" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J58" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J58" t="s">
+    <row r="59" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J59" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I59">
-        <v>1</v>
-      </c>
-      <c r="J59" t="s">
+    <row r="60" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J60" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J60" s="2" t="s">
+    <row r="61" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I61">
+        <v>1</v>
+      </c>
+      <c r="J61" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I61">
-        <v>1</v>
-      </c>
-      <c r="J61" t="s">
+    <row r="62" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J62" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J62" t="s">
+    <row r="63" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J63" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J63" t="s">
+    <row r="64" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J64" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="J64" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="65" spans="9:10" x14ac:dyDescent="0.2">
       <c r="J65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="9:10" x14ac:dyDescent="0.2">
@@ -1232,20 +1241,17 @@
         <v>1</v>
       </c>
       <c r="J66" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="J67" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="67" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I67">
-        <v>1</v>
-      </c>
-      <c r="J67" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="68" spans="9:10" x14ac:dyDescent="0.2">
       <c r="J68" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="9:10" x14ac:dyDescent="0.2">
@@ -1253,7 +1259,7 @@
         <v>1</v>
       </c>
       <c r="J69" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="9:10" x14ac:dyDescent="0.2">
@@ -1261,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="J70" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>